<commit_message>
android login page responsive issue
</commit_message>
<xml_diff>
--- a/test_case_report/sprint_45.xlsx
+++ b/test_case_report/sprint_45.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\office\SymlexVPNTestCases\test_case_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDCCAA38-6E53-4402-81AF-F856E0584224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C338F1AF-AF39-46D7-AB9D-290640E6692F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -534,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -674,19 +674,25 @@
       <c r="B27" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="2"/>
+      <c r="C27" s="2">
+        <v>7246</v>
+      </c>
     </row>
     <row r="28" spans="2:3" ht="18">
       <c r="B28" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="4"/>
+      <c r="C28" s="4">
+        <v>3030</v>
+      </c>
     </row>
     <row r="29" spans="2:3" ht="18">
       <c r="B29" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C29" s="5"/>
+      <c r="C29" s="5">
+        <v>3030</v>
+      </c>
     </row>
     <row r="32" spans="2:3" ht="18">
       <c r="B32" s="6" t="s">
@@ -810,16 +816,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B57:C57"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B57:C57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>